<commit_message>
Update example and debug messages
</commit_message>
<xml_diff>
--- a/demoExample.xlsx
+++ b/demoExample.xlsx
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikAntonelli\Planview\Development\Replicator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE0B6C0-39CF-4A61-9AA0-B04B2D7BA6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B54F94C7-C932-4E70-9A3F-E08031D8327B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="2790" windowWidth="26805" windowHeight="11385" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
+    <sheet name="C_Portfolio" sheetId="30" r:id="rId2"/>
+    <sheet name="Portfolio" sheetId="31" r:id="rId3"/>
+    <sheet name="C_Avengers ART" sheetId="32" r:id="rId4"/>
+    <sheet name="Avengers ART" sheetId="33" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="60">
   <si>
     <t>https://nacl.leankit.com/</t>
   </si>
@@ -62,10 +66,127 @@
     <t>dstApiKey</t>
   </si>
   <si>
-    <t>Portfolio 2</t>
-  </si>
-  <si>
-    <t>Avengers ART 2</t>
+    <t/>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Item Row</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>srcID</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>plannedStart</t>
+  </si>
+  <si>
+    <t>plannedFinish</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>lane</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>customId</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>blockReason</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>assignedUsers</t>
+  </si>
+  <si>
+    <t>customIcon</t>
+  </si>
+  <si>
+    <t>externalLink</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Parent Business Feature 1</t>
+  </si>
+  <si>
+    <t>31512109600139</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>#8B8EF7</t>
+  </si>
+  <si>
+    <t>Child Risk/Issue</t>
+  </si>
+  <si>
+    <t>31512110468444</t>
+  </si>
+  <si>
+    <t>Risk / Issue</t>
+  </si>
+  <si>
+    <t>#FAD7B2</t>
+  </si>
+  <si>
+    <t>31512110468879</t>
+  </si>
+  <si>
+    <t>31512110468446</t>
+  </si>
+  <si>
+    <t>31512110469256</t>
+  </si>
+  <si>
+    <t>Program Backlog^Next PI</t>
+  </si>
+  <si>
+    <t>Not Started - Future Work^New Requests</t>
+  </si>
+  <si>
+    <t>Modify</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>31512112118181</t>
   </si>
   <si>
     <t>Import Ignore</t>
@@ -74,19 +195,28 @@
     <t>Epic, Initiative</t>
   </si>
   <si>
+    <t>Epic</t>
+  </si>
+  <si>
+    <t>31512112124421</t>
+  </si>
+  <si>
+    <t>31512112124600</t>
+  </si>
+  <si>
+    <t>31512112124992</t>
+  </si>
+  <si>
+    <t>31512112124423</t>
+  </si>
+  <si>
+    <t>Target Id</t>
+  </si>
+  <si>
+    <t>325</t>
+  </si>
+  <si>
     <t>key1</t>
-  </si>
-  <si>
-    <t>key2</t>
-  </si>
-  <si>
-    <t>key3</t>
-  </si>
-  <si>
-    <t>https://somewhere.leankit.com/</t>
-  </si>
-  <si>
-    <t>https://nowhere.leankit.com/</t>
   </si>
 </sst>
 </file>
@@ -122,13 +252,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +576,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8956648B-9D53-4106-86E5-E5D70ED07D8B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,12 +587,13 @@
     <col min="1" max="2" width="49.140625" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="21.5703125" style="2" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.7109375" style="4" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="16" style="2" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="28.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -473,17 +606,20 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -491,22 +627,26 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <f>_xlfn.TEXTJOIN(,,B2," (",H2,")")</f>
+        <v>Portfolio (325)</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H2" s="5">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -514,20 +654,524 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="str">
+        <f>_xlfn.TEXTJOIN(,,B3," (",H3,")")</f>
+        <v>Avengers ART (325)</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>59</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="str">
+        <f>Portfolio!C2</f>
+        <v>Parent Business Feature 1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="18" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="str">
+        <f>'Avengers ART'!C2</f>
+        <v>Child Risk/Issue</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="str">
+        <f>'Avengers ART'!C3</f>
+        <v>Child Risk/Issue</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="str">
+        <f>'Avengers ART'!C4</f>
+        <v>Child Risk/Issue</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" t="str">
+        <f>'Avengers ART'!C5</f>
+        <v>Child Risk/Issue</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6" t="str">
+        <f>'Avengers ART'!C2</f>
+        <v>Child Risk/Issue</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="str">
+        <f>Portfolio!C2</f>
+        <v>Parent Business Feature 1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:R5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="18" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix lack of row increment when doing parents
</commit_message>
<xml_diff>
--- a/demoExample.xlsx
+++ b/demoExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikAntonelli\Planview\Development\Replicator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B54F94C7-C932-4E70-9A3F-E08031D8327B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B03EF60-834F-4759-8259-320ECBCFF7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="2790" windowWidth="26805" windowHeight="11385" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="25995" windowHeight="12840" xr2:uid="{29CD428F-0A07-48A0-8573-8048C934683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -579,7 +579,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E3" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,8 +633,8 @@
         <v>0</v>
       </c>
       <c r="E2" s="4" t="str">
-        <f>_xlfn.TEXTJOIN(,,B2," (",H2,")")</f>
-        <v>Portfolio (325)</v>
+        <f>B2&amp;"  "&amp;H2</f>
+        <v>Portfolio  325</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>59</v>
@@ -660,8 +660,8 @@
         <v>0</v>
       </c>
       <c r="E3" s="4" t="str">
-        <f>_xlfn.TEXTJOIN(,,B3," (",H3,")")</f>
-        <v>Avengers ART (325)</v>
+        <f>B3&amp;"  "&amp;H3</f>
+        <v>Avengers ART  325</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>59</v>

</xml_diff>